<commit_message>
Further changes to framework, js-files
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8E2BC6-FD35-4C6B-99D6-DF1E41887591}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0982F6-E481-48C9-B1AD-604AEEA3E8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="226">
   <si>
     <t>clause</t>
   </si>
@@ -681,12 +681,33 @@
   </si>
   <si>
     <t>A ID foi copiada para o cartão de vacinação</t>
+  </si>
+  <si>
+    <t>MIF</t>
+  </si>
+  <si>
+    <t>MIF_VISIT</t>
+  </si>
+  <si>
+    <t>Core MIF</t>
+  </si>
+  <si>
+    <t>MIF visit</t>
+  </si>
+  <si>
+    <t>MIF visita</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('MIF')</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('MIF_VISIT')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -754,7 +775,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -764,19 +785,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{1E801ADC-8186-40BD-B547-DD113501D6BA}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1057,17 +1077,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1082,20 +1102,20 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1115,7 +1135,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1123,7 +1143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1131,15 +1151,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>27052020</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20230729</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1150,7 +1170,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>171</v>
       </c>
@@ -1161,7 +1181,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>195</v>
       </c>
@@ -1172,13 +1192,13 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="10"/>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1187,21 +1207,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>172</v>
       </c>
@@ -1215,7 +1235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>190</v>
       </c>
@@ -1229,7 +1249,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>190</v>
       </c>
@@ -1243,7 +1263,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>190</v>
       </c>
@@ -1257,7 +1277,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>190</v>
       </c>
@@ -1269,6 +1289,34 @@
       </c>
       <c r="D5" t="s">
         <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -1278,24 +1326,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>174</v>
       </c>
@@ -1318,7 +1366,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>180</v>
       </c>
@@ -1326,7 +1374,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>182</v>
       </c>
@@ -1337,12 +1385,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>184</v>
       </c>
@@ -1350,22 +1398,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>213</v>
       </c>
@@ -1376,17 +1424,17 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>214</v>
       </c>
@@ -1397,17 +1445,17 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>215</v>
       </c>
@@ -1418,17 +1466,17 @@
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18" s="4" t="s">
         <v>216</v>
       </c>
@@ -1439,16 +1487,52 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E21" t="s">
+        <v>188</v>
+      </c>
+      <c r="G21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E24" t="s">
+        <v>188</v>
+      </c>
+      <c r="G24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>187</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1459,312 +1543,312 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="43.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.81640625" customWidth="1"/>
+    <col min="3" max="3" width="56.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>81</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1774,322 +1858,322 @@
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>96</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>103</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>109</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>112</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" t="s">
         <v>113</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>121</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>124</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" t="s">
         <v>125</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" t="s">
         <v>128</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" t="s">
         <v>131</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>133</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>136</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" t="s">
         <v>137</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>139</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" t="s">
         <v>140</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>142</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" t="s">
         <v>87</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>143</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" t="s">
         <v>144</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>146</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" t="s">
         <v>147</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>149</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" t="s">
         <v>150</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>152</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" t="s">
         <v>153</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
options for OOP interviews
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF22D1A-B809-4A26-B983-04787BD7E80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7922BD-80D0-4B57-A661-A457736E0517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -1092,7 +1092,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1227,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1360,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
OOP Vaccines + constraint corrections
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7922BD-80D0-4B57-A661-A457736E0517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BE8FEA-C940-491A-B003-72108CCB06AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="234">
   <si>
     <t>clause</t>
   </si>
@@ -719,7 +719,13 @@
     <t>MIF_V_OOP_ANC</t>
   </si>
   <si>
-    <t>'?' + odkSurvey.getHashString('MIF_V_ANC')</t>
+    <t>'?' + odkSurvey.getHashString('MIF_V_OOP_ANC')</t>
+  </si>
+  <si>
+    <t>MIF_V_OOP_VAC</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('MIF_V_OOP_VAC')</t>
   </si>
 </sst>
 </file>
@@ -1091,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1225,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1351,6 +1357,20 @@
         <v>229</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D9" t="s">
+        <v>229</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1358,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1605,6 +1625,27 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B33" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E33" t="s">
+        <v>188</v>
+      </c>
+      <c r="G33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
         <v>187</v>
       </c>
     </row>

</xml_diff>